<commit_message>
renaming things and better formatting
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB\Desktop\mcdaniel\constrained-k-means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EFA00C9-1E06-4A14-B958-9744C3E7CDE1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{725A34C5-A50D-48D4-A2E0-6718AA66C989}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Main" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$AJ$48</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Main!$A$1:$AJ$48</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +33,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{A459D7EA-11D4-42F2-8CD6-1132752EEA4B}" keepAlive="1" name="Query - soybean-small" description="Connection to the 'soybean-small' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Query - soybean-small" description="Connection to the 'soybean-small' query in the workbook." type="5" refreshedVersion="6" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=soybean-small;Extended Properties=&quot;&quot;" command="SELECT * FROM [soybean-small]"/>
   </connection>
 </connections>
@@ -168,7 +166,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,7 +221,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{00FD7CE6-460B-499C-BB80-C8367AD40051}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ExternalData_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="37">
     <queryTableFields count="36">
       <queryTableField id="1" name="Column1" tableColumnId="1"/>
@@ -268,45 +266,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70DE683D-A3FA-45A4-9B54-2347275AEF4E}" name="soybean_small" displayName="soybean_small" ref="A1:AJ48" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:AJ48" xr:uid="{FC0CDDB2-7055-42B2-9445-9BF99675D106}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="soybean_small" displayName="soybean_small" ref="A1:AJ48" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:AJ48"/>
   <tableColumns count="36">
-    <tableColumn id="1" xr3:uid="{03E4C01A-C083-491C-BC1E-C67C38431F18}" uniqueName="1" name="Column1" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{8F0B90A4-B94B-434A-B9EF-3E8A4117935C}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{0EB7C2FC-2A44-441E-BB7C-D7BC33DD7AC6}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
-    <tableColumn id="4" xr3:uid="{CA9B240B-4746-4441-8637-18282C71542D}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
-    <tableColumn id="5" xr3:uid="{694AB894-3DE0-4CB3-8785-A55CB424A799}" uniqueName="5" name="Column5" queryTableFieldId="5"/>
-    <tableColumn id="6" xr3:uid="{7A2FEFFA-6F53-43FF-9342-C9F4A069A99B}" uniqueName="6" name="Column6" queryTableFieldId="6"/>
-    <tableColumn id="7" xr3:uid="{7E0F1D14-8E0D-49F8-8DB5-5C62A5D626F2}" uniqueName="7" name="Column7" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{A59C4C1D-2BD1-4346-A52E-D1E3E94FDD8C}" uniqueName="8" name="Column8" queryTableFieldId="8"/>
-    <tableColumn id="9" xr3:uid="{673CE140-9FDC-4D3D-9007-C8CF6D6F6C8B}" uniqueName="9" name="Column9" queryTableFieldId="9"/>
-    <tableColumn id="10" xr3:uid="{2B14648B-16D9-4E85-8BB8-7D59C2890C4F}" uniqueName="10" name="Column10" queryTableFieldId="10"/>
-    <tableColumn id="11" xr3:uid="{30382127-7424-46FE-8023-1D4BDC5DE263}" uniqueName="11" name="Column11" queryTableFieldId="11"/>
-    <tableColumn id="12" xr3:uid="{1437FA42-FF73-4FD6-B6DB-C5BC781B8CE8}" uniqueName="12" name="Column12" queryTableFieldId="12"/>
-    <tableColumn id="13" xr3:uid="{B8C17F80-BD9C-4462-8359-1F52E568B148}" uniqueName="13" name="Column13" queryTableFieldId="13"/>
-    <tableColumn id="14" xr3:uid="{0F1F8FD1-EDE9-4929-8471-68E8D9EEC0EA}" uniqueName="14" name="Column14" queryTableFieldId="14"/>
-    <tableColumn id="15" xr3:uid="{112141A3-CF7A-4A27-9C3F-96EC6E6D281D}" uniqueName="15" name="Column15" queryTableFieldId="15"/>
-    <tableColumn id="16" xr3:uid="{9901ACC8-0BC6-4738-BB3B-8E6B28673F4B}" uniqueName="16" name="Column16" queryTableFieldId="16"/>
-    <tableColumn id="17" xr3:uid="{81295405-5500-47B1-A628-BD76B8C24B78}" uniqueName="17" name="Column17" queryTableFieldId="17"/>
-    <tableColumn id="18" xr3:uid="{A391C7D4-3A17-4A5D-9B5C-A8B5C3234703}" uniqueName="18" name="Column18" queryTableFieldId="18"/>
-    <tableColumn id="19" xr3:uid="{11AA9E93-345A-4644-83CB-52A9AD3E046B}" uniqueName="19" name="Column19" queryTableFieldId="19"/>
-    <tableColumn id="20" xr3:uid="{24B5A16F-D003-4506-BEC5-039C0C3FC8E0}" uniqueName="20" name="Column20" queryTableFieldId="20"/>
-    <tableColumn id="21" xr3:uid="{28F25534-97AB-4CCA-B7BA-F1D53D0BDFE7}" uniqueName="21" name="Column21" queryTableFieldId="21"/>
-    <tableColumn id="22" xr3:uid="{354B38F1-8036-4E0E-B4FD-00B868BCB891}" uniqueName="22" name="Column22" queryTableFieldId="22"/>
-    <tableColumn id="23" xr3:uid="{74E8544A-5B49-4A3F-BBF5-E29DB85A796F}" uniqueName="23" name="Column23" queryTableFieldId="23"/>
-    <tableColumn id="24" xr3:uid="{051451DE-65E2-4E06-B1F2-AE695348248B}" uniqueName="24" name="Column24" queryTableFieldId="24"/>
-    <tableColumn id="25" xr3:uid="{1D72E205-B484-4CEB-98FD-586076FEE8BF}" uniqueName="25" name="Column25" queryTableFieldId="25"/>
-    <tableColumn id="26" xr3:uid="{A703C8CA-C466-45C1-BA3D-4E2D2F99B566}" uniqueName="26" name="Column26" queryTableFieldId="26"/>
-    <tableColumn id="27" xr3:uid="{5F704F4E-706B-4518-A05C-86C9FCE57A9F}" uniqueName="27" name="Column27" queryTableFieldId="27"/>
-    <tableColumn id="28" xr3:uid="{AFA6CE87-68CD-4179-867F-FE2AD19BBD53}" uniqueName="28" name="Column28" queryTableFieldId="28"/>
-    <tableColumn id="29" xr3:uid="{0C365A0F-2013-473E-98C1-393B0DD7EEE7}" uniqueName="29" name="Column29" queryTableFieldId="29"/>
-    <tableColumn id="30" xr3:uid="{CD74DAC0-7BF9-48DF-BD97-0913133D8AB3}" uniqueName="30" name="Column30" queryTableFieldId="30"/>
-    <tableColumn id="31" xr3:uid="{893D4BCE-5972-44F5-BF50-E560E05E2FA5}" uniqueName="31" name="Column31" queryTableFieldId="31"/>
-    <tableColumn id="32" xr3:uid="{CA194FB1-545C-449D-8A88-3EAAD9E5E12A}" uniqueName="32" name="Column32" queryTableFieldId="32"/>
-    <tableColumn id="33" xr3:uid="{3C5695C2-CE10-4AB0-8BEC-47E1B28C6BC7}" uniqueName="33" name="Column33" queryTableFieldId="33"/>
-    <tableColumn id="34" xr3:uid="{A2279A73-AF8F-430A-987C-1351B47D61AE}" uniqueName="34" name="Column34" queryTableFieldId="34"/>
-    <tableColumn id="35" xr3:uid="{47401B29-2E75-4A29-96E0-ECB9E73EAE98}" uniqueName="35" name="Column35" queryTableFieldId="35"/>
-    <tableColumn id="36" xr3:uid="{D35A196F-6572-47A5-B085-0769AFC13966}" uniqueName="36" name="Column36" queryTableFieldId="36" dataDxfId="0"/>
+    <tableColumn id="1" uniqueName="1" name="Column1" queryTableFieldId="1"/>
+    <tableColumn id="2" uniqueName="2" name="Column2" queryTableFieldId="2"/>
+    <tableColumn id="3" uniqueName="3" name="Column3" queryTableFieldId="3"/>
+    <tableColumn id="4" uniqueName="4" name="Column4" queryTableFieldId="4"/>
+    <tableColumn id="5" uniqueName="5" name="Column5" queryTableFieldId="5"/>
+    <tableColumn id="6" uniqueName="6" name="Column6" queryTableFieldId="6"/>
+    <tableColumn id="7" uniqueName="7" name="Column7" queryTableFieldId="7"/>
+    <tableColumn id="8" uniqueName="8" name="Column8" queryTableFieldId="8"/>
+    <tableColumn id="9" uniqueName="9" name="Column9" queryTableFieldId="9"/>
+    <tableColumn id="10" uniqueName="10" name="Column10" queryTableFieldId="10"/>
+    <tableColumn id="11" uniqueName="11" name="Column11" queryTableFieldId="11"/>
+    <tableColumn id="12" uniqueName="12" name="Column12" queryTableFieldId="12"/>
+    <tableColumn id="13" uniqueName="13" name="Column13" queryTableFieldId="13"/>
+    <tableColumn id="14" uniqueName="14" name="Column14" queryTableFieldId="14"/>
+    <tableColumn id="15" uniqueName="15" name="Column15" queryTableFieldId="15"/>
+    <tableColumn id="16" uniqueName="16" name="Column16" queryTableFieldId="16"/>
+    <tableColumn id="17" uniqueName="17" name="Column17" queryTableFieldId="17"/>
+    <tableColumn id="18" uniqueName="18" name="Column18" queryTableFieldId="18"/>
+    <tableColumn id="19" uniqueName="19" name="Column19" queryTableFieldId="19"/>
+    <tableColumn id="20" uniqueName="20" name="Column20" queryTableFieldId="20"/>
+    <tableColumn id="21" uniqueName="21" name="Column21" queryTableFieldId="21"/>
+    <tableColumn id="22" uniqueName="22" name="Column22" queryTableFieldId="22"/>
+    <tableColumn id="23" uniqueName="23" name="Column23" queryTableFieldId="23"/>
+    <tableColumn id="24" uniqueName="24" name="Column24" queryTableFieldId="24"/>
+    <tableColumn id="25" uniqueName="25" name="Column25" queryTableFieldId="25"/>
+    <tableColumn id="26" uniqueName="26" name="Column26" queryTableFieldId="26"/>
+    <tableColumn id="27" uniqueName="27" name="Column27" queryTableFieldId="27"/>
+    <tableColumn id="28" uniqueName="28" name="Column28" queryTableFieldId="28"/>
+    <tableColumn id="29" uniqueName="29" name="Column29" queryTableFieldId="29"/>
+    <tableColumn id="30" uniqueName="30" name="Column30" queryTableFieldId="30"/>
+    <tableColumn id="31" uniqueName="31" name="Column31" queryTableFieldId="31"/>
+    <tableColumn id="32" uniqueName="32" name="Column32" queryTableFieldId="32"/>
+    <tableColumn id="33" uniqueName="33" name="Column33" queryTableFieldId="33"/>
+    <tableColumn id="34" uniqueName="34" name="Column34" queryTableFieldId="34"/>
+    <tableColumn id="35" uniqueName="35" name="Column35" queryTableFieldId="35"/>
+    <tableColumn id="36" uniqueName="36" name="Column36" queryTableFieldId="36" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -608,10 +606,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC7727C-FB3B-4583-B7FE-E369DF42AEA2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -5906,18 +5904,6 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03C89080-DDC6-4456-989F-D86940194DB5}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>